<commit_message>
All auc values extracted
</commit_message>
<xml_diff>
--- a/RiboApplication/excelTables/modelsAocValuesTable.xlsx
+++ b/RiboApplication/excelTables/modelsAocValuesTable.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="sklearn" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="RnnClassifierModel" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,43 +370,13 @@
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -414,22 +384,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -437,22 +392,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -460,22 +400,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -483,22 +408,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -506,21 +416,6 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="G7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -529,22 +424,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -552,22 +432,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -575,22 +440,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -598,21 +448,6 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="G11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -621,22 +456,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -644,21 +464,6 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="G13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -667,21 +472,6 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -690,21 +480,6 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="G15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -713,22 +488,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -736,22 +496,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -759,22 +504,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -782,22 +512,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -805,22 +520,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -828,21 +528,6 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="G21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -851,21 +536,6 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -874,21 +544,6 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="G23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -897,21 +552,6 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="G24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -920,21 +560,6 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="F25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -943,21 +568,6 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="G26" t="n">
         <v>1</v>
       </c>
     </row>
@@ -966,22 +576,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>